<commit_message>
minor changes on driver
</commit_message>
<xml_diff>
--- a/news_data.xlsx
+++ b/news_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5 hours ago ... ...AIsys­tems in its de­struc­tion of Gaza. The ex­perts were re­spond­ing to re­ports Is­rael is us­ing AI sys­tems known as the “Gospel”, “Laven­der ...</t>
+          <t>8 hours ago ... ...AIsys­tems in its de­struc­tion of Gaza. The ex­perts were re­spond­ing to re­ports Is­rael is us­ing AI sys­tems known as the “Gospel”, “Laven­der ...</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -492,7 +492,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14 hours ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. The ads do not meet the lev­els of dis­clo­sure Meta says it needs for AI-gen­er­at­ed ...</t>
+          <t>16 hours ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. The ads do not meet the lev­els of dis­clo­sure Meta says it needs for AI-gen­er­at­ed ...</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,13 +512,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Econ­o­my | To­day's lat­est from Al Jazeera</t>
+          <t>Iran | To­day's lat­est from Al Jazeera</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14 hours ago ... The ads do not meet the lev­els of dis­clo­sure Meta says it needs forAI-gen­er­at­ed posts linked to In­dia elec­tion. Pub­lished On 12 Apr 202412 Apr 2024. In­di­an ...</t>
+          <t>16 hours ago ... Is­raeli 'diplo­mat­ic of­fen­sive' urges sanc­tions against Iran ... Push on part­ners to sanc­tion Tehran comes as Is­rael mulls mil­i­tary re­tal­i­a­tion for Iran's week­end ...</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -538,17 +538,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tes­la to lay off more than 10 per­cent of staff world­wide amid falling ...</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16 Apr 2024</t>
-        </is>
-      </c>
+          <t>Econ­o­my | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>13 hours ago ... ... ar­ti­fi­cial in­tel­li­gence”. In a post on X af­ter the news be­came pub­lic, Musk said that Tes­la need­ed to “re­or­gan­ise and stream­line the com­pa­ny ...</t>
+          <t>16 hours ago ... The ads do not meet the lev­els of dis­clo­sure Meta says it needs forAI-gen­er­at­ed posts linked to In­dia elec­tion. Pub­lished On 12 Apr 202412 Apr 2024. In­di­an ...</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -568,13 +564,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>News | To­day's lat­est from Al Jazeera</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>Tes­la to lay off more than 10 per­cent of staff world­wide amid falling ...</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>16 Apr 2024</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14 hours ago ... Is Ukraine's Za­phorizhzhia nu­clear plant at risk of an 'ac­ci­den­t'? Glob­al pow­ers raise alarm af­ter lat­est drone at­tack on Russ­ian-held nu­clear fa­cil­i­ty hits ...</t>
+          <t>15 hours ago ... ... ar­ti­fi­cial in­tel­li­gence”. In a post on X af­ter the news be­came pub­lic, Musk said that Tes­la need­ed to “re­or­gan­ise and stream­line the com­pa­ny ...</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -594,13 +594,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Break­ing News, World News and Video from Al Jazeera</t>
+          <t>News | To­day's lat­est from Al Jazeera</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8 hours ago ... News, analy­sis from the Mid­dle East &amp; world­wide, mul­ti­me­dia &amp; in­ter­ac­tives, opin­ions, doc­u­men­taries, pod­casts, long reads and broad­cast ...</t>
+          <t>16 hours ago ... Is Ukraine's Za­phorizhzhia nu­clear plant at risk of an 'ac­ci­den­t'? Glob­al pow­ers raise alarm af­ter lat­est drone at­tack on Russ­ian-held nu­clear fa­cil­i­ty hits ...</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -620,13 +620,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fea­tures | To­day's lat­est from Al Jazeera</t>
+          <t>Break­ing News, World News and Video from Al Jazeera</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14 hours ago ... Stay on top of Fea­tures lat­est de­vel­op­ments on the ground with Al Jazeer­a's fact-based news, ex­clu­sive video footage, pho­tos and up­dat­ed maps.</t>
+          <t>1 hour ago ... News, analy­sis from the Mid­dle East &amp; world­wide, mul­ti­me­dia &amp; in­ter­ac­tives, opin­ions, doc­u­men­taries, pod­casts, long reads and broad­cast ...</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -646,17 +646,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chat­G­PT ri­val 'Ernie Bot' now has 200 mil­lion users, Chi­na's Baidu ...</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16 Apr 2024</t>
-        </is>
-      </c>
+          <t>Fea­tures | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9 hours ago ... Re­cent data shows that ri­val do­mes­ticAIser­vices, par­tic­u­lar­ly the “Kimi” chat­bot from a 12-month-old Al­iba­ba-backed start-up named Moon­shot AI ...</t>
+          <t>16 hours ago ... Stay on top of Fea­tures lat­est de­vel­op­ments on the ground with Al Jazeer­a's fact-based news, ex­clu­sive video footage, pho­tos and up­dat­ed maps.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -665,7 +661,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -676,17 +672,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Birth, death, es­cape: Three wom­en's strug­gle through Su­dan's war ...</t>
+          <t>Chat­G­PT ri­val 'Ernie Bot' now has 200 mil­lion users, Chi­na's Baidu ...</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15 Apr 2024</t>
+          <t>16 Apr 2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1 day ago ... ThisAI-gen­er­at­ed pho­to is for rep­re­sen­ta­tion­al pur­pos­es only and used to pre­serve the in­di­vid­u­al's safe­ty [Al Jazeera]. By Mat Nashed.</t>
+          <t>11 hours ago ... Re­cent data shows that ri­val do­mes­ticAIser­vices, par­tic­u­lar­ly the “Kimi” chat­bot from a 12-month-old Al­iba­ba-backed start-up named Moon­shot AI ...</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -695,7 +691,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -706,13 +702,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Con­flict | To­day's lat­est from Al Jazeera</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+          <t>Birth, death, es­cape: Three wom­en's strug­gle through Su­dan's war ...</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>15 Apr 2024</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2 days ago ... Stay on top of Con­flict lat­est de­vel­op­ments on the ground with Al Jazeer­a's fact-based news, ex­clu­sive video footage, pho­tos and up­dat­ed maps.</t>
+          <t>1 day ago ... ThisAI-gen­er­at­ed pho­to is for rep­re­sen­ta­tion­al pur­pos­es only and used to pre­serve the in­di­vid­u­al's safe­ty [Al Jazeera]. By Mat Nashed.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -768,7 +768,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>18 hours ago ... Geno­cide in Gaza: En­abled byAI, pow­ered by Big Tech. Ar­ti­fi­cial in­tel­li­gence has un­leashed ter­ror in the killing fields of Gaza. Video ...</t>
+          <t>21 hours ago ... Geno­cide in Gaza: En­abled byAI, pow­ered by Big Tech. Ar­ti­fi­cial in­tel­li­gence has un­leashed ter­ror in the killing fields of Gaza. Video ...</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -809,7 +809,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mod­i's elec­tions or Dic­ta­tor Aladeen's Olympics? | In­dia Elec­tion ...</t>
+          <t>Stocks slide on Mid­dle East ten­sions as hope cri­sis con­tained stems ...</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -819,7 +819,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>23 hours ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules ... Sure, In­dia can­not for­mal­ly be clas­si­fied as a dic­ta­tor­ship, but it ...</t>
+          <t>1 day ago ... Japan's Nikkei stock in­dex pass­es 40,000 for first time amidAIfan­fare. Nikkei 225 gains as much as 1 per­cent af­ter last month beat­ing 1989 ...</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -839,17 +839,13 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Stocks slide on Mid­dle East ten­sions as hope cri­sis con­tained stems ...</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>15 Apr 2024</t>
-        </is>
-      </c>
+          <t>Opin­ion | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1 day ago ... Japan's Nikkei stock in­dex pass­es 40,000 for first time amidAIfan­fare. Nikkei 225 gains as much as 1 per­cent af­ter last month beat­ing 1989 ...</t>
+          <t>3 days ago ... Stay on top of Opin­ion lat­est de­vel­op­ments on the ground with Al Jazeer­a's fact-based news, ex­clu­sive video footage, pho­tos and up­dat­ed maps.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -858,7 +854,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1019,13 +1015,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Qatar | To­day's lat­est from Al Jazeera</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
+          <t>As Rus­si­a's war rages, Ukraine's men­tal health cri­sis spi­rals | Rus­sia ...</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11 Apr 2024</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6 days ago ...AItakes cen­tre stage as Web Sum­mit kicks off in Qatar. Held in the Mid­dle East for the first time, the tech­nol­o­gy con­fer­ence aims to con­nect en­tre­pre­neurs with ...</t>
+          <t>5 days ago ... Writ­ing a di­ary was an ini­tial cop­ing mech­a­nism for Ole­na Kuk, 27, a TV pre­sen­ter and com­mu­ni­ca­tion spe­cial­ist at theAIFor Good Foun­da­tion, ...</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1045,17 +1045,13 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Will ul­tra-Or­tho­dox Jews have to en­list in the Is­raeli army? | Protests ...</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11 Apr 2024</t>
-        </is>
-      </c>
+          <t>Qatar | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>5 days ago ... 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. end of list. Last week, with Is­rael's coali­tion gov­ern­ment un­able ...</t>
+          <t>6 days ago ...AItakes cen­tre stage as Web Sum­mit kicks off in Qatar. Held in the Mid­dle East for the first time, the tech­nol­o­gy con­fer­ence aims to con­nect en­tre­pre­neurs with ...</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1064,7 +1060,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1075,7 +1071,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sin­ga­pore tight­ens rules for ex­pat work­ers with an eye on lo­cal ...</t>
+          <t>Will ul­tra-Or­tho­dox Jews have to en­list in the Is­raeli army? | Protests ...</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1085,7 +1081,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6 days ago ... ...AI, tech­nol­o­gy, en­gi­neer­ing and health­care. “The trend of lim­it­ing for­eign tal­ent de­ploy­ment to spe­cif­ic skills and in­dus­tries is in­evitable ...</t>
+          <t>5 days ago ... 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. end of list. Last week, with Is­rael's coali­tion gov­ern­ment un­able ...</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1105,7 +1101,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Will oil prices keep ris­ing, and how will that af­fect in­fla­tion ...</t>
+          <t>Sin­ga­pore tight­ens rules for ex­pat work­ers with an eye on lo­cal ...</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1115,7 +1111,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>5 days ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. list 4 of 4. Sin­ga­pore 'tight­ens screws' on Myan­mar gen­er­als with ...</t>
+          <t>6 days ago ... ...AI, tech­nol­o­gy, en­gi­neer­ing and health­care. “The trend of lim­it­ing for­eign tal­ent de­ploy­ment to spe­cif­ic skills and in­dus­tries is in­evitable ...</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1135,17 +1131,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Eu­ro­pean Par­lia­ment pass­es asy­lum and mi­gra­tion re­forms ...</t>
+          <t>Will oil prices keep ris­ing, and how will that af­fect in­fla­tion ...</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>10 Apr 2024</t>
+          <t>11 Apr 2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>6 days ago ... Eu­ro­pean Union reach­es agree­ment on land­mark leg­is­la­tion to reg­u­lateAI. list 3 of 3. The EU's se­cret weapon against refugees — time. end of ...</t>
+          <t>5 days ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. list 4 of 4. Sin­ga­pore 'tight­ens screws' on Myan­mar gen­er­als with ...</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1154,7 +1150,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1165,7 +1161,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Rat­ings agency Fitch low­ers Chi­na's sov­er­eign cred­it out­look to ...</t>
+          <t>Eu­ro­pean Par­lia­ment pass­es asy­lum and mi­gra­tion re­forms ...</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1175,7 +1171,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>6 days ago ... Chi­nese state me­di­a's A Frac­tured Amer­i­ca se­ries shows howAIis be­gin­ning to shape Bei­jing's in­flu­ence cam­paigns. Pub­lished On 29 Mar 202429 ...</t>
+          <t>6 days ago ... Eu­ro­pean Union reach­es agree­ment on land­mark leg­is­la­tion to reg­u­lateAI. list 3 of 3. The EU's se­cret weapon against refugees — time. end of ...</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1195,13 +1191,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Iraq | To­day's lat­est from Al Jazeera</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
+          <t>Rat­ings agency Fitch low­ers Chi­na's sov­er­eign cred­it out­look to ...</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>10 Apr 2024</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>8 days ago ... Arab na­tions had closed air­spaces af­ter Iran's drone and mis­sile at­tacks on Is­rael, but many flights re­main af­fect­ed. Pub­lished On 14 Apr 202414 Apr 2024.</t>
+          <t>6 days ago ... Chi­nese state me­di­a's A Frac­tured Amer­i­ca se­ries shows howAIis be­gin­ning to shape Bei­jing's in­flu­ence cam­paigns. Pub­lished On 29 Mar 202429 ...</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1221,17 +1221,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Biden un­veils $6.6bn for Tai­wan's TSMC to ramp up US chip ...</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>09 Apr 2024</t>
-        </is>
-      </c>
+          <t>Iraq | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>8 days ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. AI-gen­er­at­ed im­ages of In­di­an Prime Min­is­ter Naren­dra Modi are be­ing ...</t>
+          <t>8 days ago ... Arab na­tions had closed air­spaces af­ter Iran's drone and mis­sile at­tacks on Is­rael, but many flights re­main af­fect­ed. Pub­lished On 14 Apr 202414 Apr 2024.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1240,18 +1236,18 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Why a Sri Lankan is­land is spark­ing an In­di­an elec­tion con­tro­ver­sy ...</t>
+          <t>Biden un­veils $6.6bn for Tai­wan's TSMC to ramp up US chip ...</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1270,28 +1266,28 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Pak­istan's del­i­cate ban­gles that make Eid al-Fitr out­fits 'com­plete' | In ...</t>
+          <t>Why a Sri Lankan is­land is spark­ing an In­di­an elec­tion con­tro­ver­sy ...</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>08 Apr 2024</t>
+          <t>09 Apr 2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Apr 7, 2024 ... It wants reg­u­la­tion to pro­tect mod­els so brands, agen­cies don't useAIto cre­ate dig­i­tal repli­cas with­out con­sent. Pub­lished On 23 Feb 2024 ...</t>
+          <t>8 days ago ... Be­fore In­dia elec­tion, In­sta­gram boosts ModiAIim­ages that vi­o­late rules. AI-gen­er­at­ed im­ages of In­di­an Prime Min­is­ter Naren­dra Modi are be­ing ...</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1300,7 +1296,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1311,17 +1307,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Is­rael's war on Gaza – six re­lent­less months of death and de­struc­tion ...</t>
+          <t>Pak­istan's del­i­cate ban­gles that make Eid al-Fitr out­fits 'com­plete' | In ...</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>07 Apr 2024</t>
+          <t>08 Apr 2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Apr 6, 2024 ... Keep read­ing · 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists · Gaza aid work­er killings are a 'mes­sage to the world'.</t>
+          <t>Apr 7, 2024 ... It wants reg­u­la­tion to pro­tect mod­els so brands, agen­cies don't useAIto cre­ate dig­i­tal repli­cas with­out con­sent. Pub­lished On 23 Feb 2024 ...</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1330,7 +1326,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1341,17 +1337,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pelosi joins US De­moc­rats call for Biden to halt arms trans­fer to ...</t>
+          <t>Is­rael's war on Gaza – six re­lent­less months of death and de­struc­tion ...</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06 Apr 2024</t>
+          <t>07 Apr 2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Apr 5, 2024 ... Keep read­ing. list of 4 items list 1 of 4. 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. list 2 of 4. Is­rael to ...</t>
+          <t>Apr 6, 2024 ... Keep read­ing · 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists · Gaza aid work­er killings are a 'mes­sage to the world'.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1360,7 +1356,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1371,7 +1367,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Re­port­ing un­der geno­cide: Six months in Gaza | TV Shows | Al ...</t>
+          <t>Pelosi joins US De­moc­rats call for Biden to halt arms trans­fer to ...</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1381,7 +1377,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Apr 5, 2024 ... More from the same show · Geno­cide in Gaza: En­abled byAI, pow­ered by Big Tech · The cracks are deep­en­ing in the US-Is­rael al­liance · Dis­sect­ing ...</t>
+          <t>Apr 5, 2024 ... Keep read­ing. list of 4 items list 1 of 4. 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. list 2 of 4. Is­rael to ...</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1401,7 +1397,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Is­raeli fire 'most like­ly' killed woman tak­en cap­tive on Oc­to­ber 7 ...</t>
+          <t>Re­port­ing un­der geno­cide: Six months in Gaza | TV Shows | Al ...</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1411,7 +1407,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Apr 4, 2024 ... This week, me­dia re­ports shone a light on theAI-as­sist­ed sys­tem Is­rael uses to iden­ti­fy tar­gets for its bomb­ing cam­paign in Gaza. The ...</t>
+          <t>Apr 5, 2024 ... More from the same show · Geno­cide in Gaza: En­abled byAI, pow­ered by Big Tech · The cracks are deep­en­ing in the US-Is­rael al­liance · Dis­sect­ing ...</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1420,7 +1416,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1431,17 +1427,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>At In­done­si­a's biggest bank, cus­tomer­s' sav­ings can van­ish with a ...</t>
+          <t>Is­raeli fire 'most like­ly' killed woman tak­en cap­tive on Oc­to­ber 7 ...</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>08 Apr 2024</t>
+          <t>06 Apr 2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Apr 4, 2024 ... The bank said it utilis­es a “com­pre­hen­sive ap­proach” to min­imise the risk of cus­tomer data breach­es, in­clud­ing us­ing ar­ti­fi­cial in­tel­li­gence (AI) ...</t>
+          <t>Apr 4, 2024 ... This week, me­dia re­ports shone a light on theAI-as­sist­ed sys­tem Is­rael uses to iden­ti­fy tar­gets for its bomb­ing cam­paign in Gaza. The ...</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1461,17 +1457,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>UN rights body de­mands Is­rael be held ac­count­able for pos­si­ble ...</t>
+          <t>At In­done­si­a's biggest bank, cus­tomer­s' sav­ings can van­ish with a ...</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>05 Apr 2024</t>
+          <t>08 Apr 2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Apr 4, 2024 ... Keep read­ing. list of 4 items list 1 of 4. 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. list 2 of 4. Is­rael to ...</t>
+          <t>Apr 4, 2024 ... The bank said it utilis­es a “com­pre­hen­sive ap­proach” to min­imise the risk of cus­tomer data breach­es, in­clud­ing us­ing ar­ti­fi­cial in­tel­li­gence (AI) ...</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1480,7 +1476,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1491,7 +1487,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Is­raeli mil­i­tary sacks two of­fi­cers over strikes on WCK aid con­voy ...</t>
+          <t>UN rights body de­mands Is­rael be held ac­count­able for pos­si­ble ...</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1501,7 +1497,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Apr 4, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets. Pub­lished On 4 Apr 20244 ...</t>
+          <t>Apr 4, 2024 ... Keep read­ing. list of 4 items list 1 of 4. 'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill lists. list 2 of 4. Is­rael to ...</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1510,7 +1506,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1521,7 +1517,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>How du­bi­ous YouTube 'news' chan­nels are boost­ing Modi in In­di­a's ...</t>
+          <t>Is­raeli mil­i­tary sacks two of­fi­cers over strikes on WCK aid con­voy ...</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1531,7 +1527,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Apr 4, 2024 ... A study done by Nar­ra­tive Re­search Lab, a New Del­hi-based data lab that uses ar­ti­fi­cial in­tel­li­gence (AI) to track print me­dia and so­cial ...</t>
+          <t>Apr 4, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets. Pub­lished On 4 Apr 20244 ...</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1540,7 +1536,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1551,17 +1547,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Is­rael boosts de­fences af­ter Iran con­sulate at­tack in Syr­ia | News | Al ...</t>
+          <t>How du­bi­ous YouTube 'news' chan­nels are boost­ing Modi in In­di­a's ...</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>04 Apr 2024</t>
+          <t>05 Apr 2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Apr 3, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets. Pub­lished On 4 Apr 20244 ...</t>
+          <t>Apr 4, 2024 ... A study done by Nar­ra­tive Re­search Lab, a New Del­hi-based data lab that uses ar­ti­fi­cial in­tel­li­gence (AI) to track print me­dia and so­cial ...</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1581,7 +1577,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill ...</t>
+          <t>Is­rael boosts de­fences af­ter Iran con­sulate at­tack in Syr­ia | News | Al ...</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1591,7 +1587,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Apr 3, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets.</t>
+          <t>Apr 3, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets. Pub­lished On 4 Apr 20244 ...</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1600,7 +1596,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1611,17 +1607,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Is­rael's war on Gaza up­dates: Biden threat­ens pol­i­cy change on ...</t>
+          <t>'AI-as­sist­ed geno­cide': Is­rael re­port­ed­ly used data­base for Gaza kill ...</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>05 Apr 2024</t>
+          <t>04 Apr 2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Apr 3, 2024 ... US look­ing at re­ports Is­rael usedAIto iden­ti­fy bomb­ing tar­gets in Gaza. The Unit­ed States is look­ing into a +972 Mag­a­zine and Lo­cal Call ...</t>
+          <t>Apr 3, 2024 ... Two Is­raeli me­dia out­lets re­port Is­raeli mil­i­tary's use ofAI-as­sist­ed sys­tem called Laven­der to iden­ti­fy Gaza tar­gets.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1630,7 +1626,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1641,17 +1637,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Will the US un­em­ploy­ment rate con­tin­ue at his­toric lows? | Busi­ness ...</t>
+          <t>Is­rael's war on Gaza up­dates: Biden threat­ens pol­i­cy change on ...</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>04 Apr 2024</t>
+          <t>05 Apr 2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Apr 3, 2024 ... Amer­i­cans are be­ing de­clined for loans, mem­ber­ships and even job op­por­tu­ni­ties byAIsys­tems with­out any ap­peal pol­i­cy. Pub­lished On 12 Feb ...</t>
+          <t>Apr 3, 2024 ... US look­ing at re­ports Is­rael usedAIto iden­ti­fy bomb­ing tar­gets in Gaza. The Unit­ed States is look­ing into a +972 Mag­a­zine and Lo­cal Call ...</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1671,17 +1667,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Ope­nAI de­buts voice cloning tool, but deems it too risky for pub­lic ...</t>
+          <t>Will the US un­em­ploy­ment rate con­tin­ue at his­toric lows? | Busi­ness ...</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>01 Apr 2024</t>
+          <t>04 Apr 2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mar 31, 2024 ... The in­flu­ence ofAIon vot­ers has al­ready come un­der scruti­ny in sev­er­al elec­tions. Pak­istan's jailed for­mer Prime Min­is­ter Im­ran Khan used AI ...</t>
+          <t>Apr 3, 2024 ... Amer­i­cans are be­ing de­clined for loans, mem­ber­ships and even job op­por­tu­ni­ties byAIsys­tems with­out any ap­peal pol­i­cy. Pub­lished On 12 Feb ...</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1690,7 +1686,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1701,17 +1697,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Chi­na turns to AI in pro­pa­gan­da mock­ing the 'Amer­i­can Dream ...</t>
+          <t>Ope­nAI de­buts voice cloning tool, but deems it too risky for pub­lic ...</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>29 Mar 2024</t>
+          <t>01 Apr 2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mar 28, 2024 ... Chi­nese state me­di­a's A Frac­tured Amer­i­ca se­ries shows howAIis be­gin­ning to shape Bei­jing's in­flu­ence cam­paigns.</t>
+          <t>Mar 31, 2024 ... The in­flu­ence ofAIon vot­ers has al­ready come un­der scruti­ny in sev­er­al elec­tions. Pak­istan's jailed for­mer Prime Min­is­ter Im­ran Khan used AI ...</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1720,7 +1716,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1731,17 +1727,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Could Ope­nAI's Sora text-to-video gen­er­a­tor kill off jobs in ...</t>
+          <t>Chi­na turns to AI in pro­pa­gan­da mock­ing the 'Amer­i­can Dream ...</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>31 Mar 2024</t>
+          <t>29 Mar 2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mar 28, 2024 ... Ar­ti­fi­cial in­tel­li­gence start­up OpenAIhas been teas­ing its new AI video gen­er­a­tor, Sora, on so­cial me­dia in re­cent weeks. Last week, it ...</t>
+          <t>Mar 28, 2024 ... Chi­nese state me­di­a's A Frac­tured Amer­i­ca se­ries shows howAIis be­gin­ning to shape Bei­jing's in­flu­ence cam­paigns.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1761,17 +1757,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fears of AI dis­in­for­ma­tion cast shad­ow over Turk­ish lo­cal elec­tions ...</t>
+          <t>Could Ope­nAI's Sora text-to-video gen­er­a­tor kill off jobs in ...</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>28 Mar 2024</t>
+          <t>31 Mar 2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mar 27, 2024 ... Turk­ish politi­cians have de­nounced the use of what they say are ma­nip­u­lat­ed im­ages and videos for elec­toral ad­van­tage.</t>
+          <t>Mar 28, 2024 ... Ar­ti­fi­cial in­tel­li­gence start­up OpenAIhas been teas­ing its new AI video gen­er­a­tor, Sora, on so­cial me­dia in re­cent weeks. Last week, it ...</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1780,7 +1776,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -1791,13 +1787,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sau­di Ara­bia | To­day's lat­est from Al Jazeera</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr"/>
+          <t>Fears of AI dis­in­for­ma­tion cast shad­ow over Turk­ish lo­cal elec­tions ...</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>28 Mar 2024</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mar 20, 2024 ... Cris­tiano Ronal­do's wait for a Sau­di Ara­bi­an foot­ball tro­phy will con­tin­ue af­ter Su­per Cup exit. ... Al Nass­r's Cris­tiano Ronal­do walks on field. WTA Fi­nals ...</t>
+          <t>Mar 27, 2024 ... Turk­ish politi­cians have de­nounced the use of what they say are ma­nip­u­lat­ed im­ages and videos for elec­toral ad­van­tage.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1817,17 +1817,13 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>UN ap­proves its first res­o­lu­tion on ar­ti­fi­cial in­tel­li­gence | Tech­nol­o­gy ...</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>22 Mar 2024</t>
-        </is>
-      </c>
+          <t>Sau­di Ara­bia | To­day's lat­est from Al Jazeera</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Mar 20, 2024 ... The UN Gen­er­al As­sem­bly has called for a set of in­ter­na­tion­al guide­lines to ad­dress the risks and ben­e­fits ofAI.</t>
+          <t>Mar 20, 2024 ... Cris­tiano Ronal­do's wait for a Sau­di Ara­bi­an foot­ball tro­phy will con­tin­ue af­ter Su­per Cup exit. ... Al Nass­r's Cris­tiano Ronal­do walks on field. WTA Fi­nals ...</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1847,17 +1843,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>French reg­u­la­tor hits Google with $272m fine over me­dia li­cens­ing ...</t>
+          <t>UN ap­proves its first res­o­lu­tion on ar­ti­fi­cial in­tel­li­gence | Tech­nol­o­gy ...</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>20 Mar 2024</t>
+          <t>22 Mar 2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Mar 19, 2024 ... The watch­dog said Google's ar­ti­fi­cial in­tel­li­gence-pow­ered chat­bot Bard – since re­brand­ed Gem­i­ni – was trained on con­tent from pub­lish­ers and ...</t>
+          <t>Mar 20, 2024 ... The UN Gen­er­al As­sem­bly has called for a set of in­ter­na­tion­al guide­lines to ad­dress the risks and ben­e­fits ofAI.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1866,28 +1862,28 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Tech gi­ant Nvidia un­veils high­er per­form­ing 'su­per­chip­s' to pow­er AI ...</t>
+          <t>French reg­u­la­tor hits Google with $272m fine over me­dia li­cens­ing ...</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>19 Mar 2024</t>
+          <t>20 Mar 2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Mar 18, 2024 ... Nvidi­a's pow­er­ful GPU chips and soft­ware are an in­te­gral in­gre­di­ent in the cre­ation of gen­er­a­tiveAI, with ri­vals like AMD or In­tel still ...</t>
+          <t>Mar 19, 2024 ... The watch­dog said Google's ar­ti­fi­cial in­tel­li­gence-pow­ered chat­bot Bard – since re­brand­ed Gem­i­ni – was trained on con­tent from pub­lish­ers and ...</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1899,6 +1895,36 @@
         <v>2</v>
       </c>
       <c r="F51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Tech gi­ant Nvidia un­veils high­er per­form­ing 'su­per­chip­s' to pow­er AI ...</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>19 Mar 2024</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Mar 18, 2024 ... Nvidi­a's pow­er­ful GPU chips and soft­ware are an in­te­gral in­gre­di­ent in the cre­ation of gen­er­a­tiveAI, with ri­vals like AMD or In­tel still ...</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>output/images/img-50</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>